<commit_message>
O problema era do limite dos campos, especificamente no campo telefone da sheet da planilha.
</commit_message>
<xml_diff>
--- a/importExcelMvc/wwwroot/Subidos/pessoasTesteUpload.xlsx
+++ b/importExcelMvc/wwwroot/Subidos/pessoasTesteUpload.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Benedito Enzo Ribeiro</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Vila de Rondônia</t>
   </si>
   <si>
-    <t>(69) 3819-7424</t>
-  </si>
-  <si>
     <t>Nome</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Beira Rio</t>
   </si>
   <si>
-    <t>(86) 2541-8136</t>
-  </si>
-  <si>
     <t>Daiane Isis Mirella Almada</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>Educandos</t>
   </si>
   <si>
-    <t>(92) 3614-4316</t>
-  </si>
-  <si>
     <t>Ricardo Marcelo Souza</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
   </si>
   <si>
     <t>Paratibe</t>
-  </si>
-  <si>
-    <t>(83) 2896-4906</t>
   </si>
 </sst>
 </file>
@@ -404,29 +392,29 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -439,50 +427,50 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
+      <c r="D2">
+        <v>6938197424</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="D3">
+        <v>8625418136</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+      <c r="D4">
+        <v>9236144316</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>8328964906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>